<commit_message>
Résultats affinés pour 2020
</commit_message>
<xml_diff>
--- a/Final_results/BDF_all_2020.xlsx
+++ b/Final_results/BDF_all_2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="439">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -755,10 +755,19 @@
     <t xml:space="preserve">2020-01-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, and you are giving a speech about the economic outlook of France. Today is 09 January 2020. Using ONLY information that was available on or before 09 January 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2019 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
+    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, giving a speech about the economic outlook of France. Today is 09 January 2020. You will be provided with a document with information about the current state and recent past of the French economy. Using ONLY the information in that document and information that was available on or before 09 January 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2019 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 09 January 2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.1 (75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.1 (85)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-02-08</t>
@@ -881,16 +890,28 @@
     <t xml:space="preserve">2020-08-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, and you are giving a speech about the economic outlook of France. Today is 09 August 2020. Using ONLY information that was available on or before 09 August 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the third quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
+    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, giving a speech about the economic outlook of France. Today is 09 August 2020. You will be provided with a document with information about the current state and recent past of the French economy. Using ONLY the information in that document and information that was available on or before 09 August 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the third quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 09 August 2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">+16.0 (65)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+16.0 (60)</t>
+    <t xml:space="preserve">
++16.0 (75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+16.0 (75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++16.0 (70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++15.7 (65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+16.0 (70)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-09-08</t>
@@ -911,56 +932,88 @@
     <t xml:space="preserve">2020-10-07</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, and you are giving a speech about the economic outlook of France. Today is 07 October 2020. Using ONLY information that was available on or before 07 October 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the third quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
+    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, giving a speech about the economic outlook of France. Today is 07 October 2020. You will be provided with a document with information about the current state and recent past of the French economy. Using ONLY the information in that document and information that was available on or before 07 October 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the third quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 07 October 2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">+16.0 (90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+18.0 (85)</t>
+    <t xml:space="preserve">
++15.0 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++15.7 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++16.0 (95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+16.0 (95)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-11-08</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, and you are giving a speech about the economic outlook of France. Today is 08 November 2020. Using ONLY information that was available on or before 08 November 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
+    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, giving a speech about the economic outlook of France. Today is 08 November 2020. You will be provided with a document with information about the current state and recent past of the French economy. Using ONLY the information in that document and information that was available on or before 08 November 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 08 November 2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">-4.0 (60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.0 (40)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.0 (50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.2 (40)</t>
+    <t xml:space="preserve">-4.2 (65)</t>
   </si>
   <si>
     <t xml:space="preserve">
--4.2 (40)</t>
+-4.2 (65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5.8 (70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-3.7 (65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-5.4 (65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-5.5 (60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5.4 (65)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-12-13</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, and you are giving a speech about the economic outlook of France. Today is 13 December 2020. Using ONLY information that was available on or before 13 December 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
+    <t xml:space="preserve">Forget the previous instructions and answers. You are François Villeroy de Galhau, Governor of the Banque de France, giving a speech about the economic outlook of France. Today is 13 December 2020. You will be provided with a document with information about the current state and recent past of the French economy. Using ONLY the information in that document and information that was available on or before 13 December 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 13 December 2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">-4.0 (75)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.0 (80)</t>
+    <t xml:space="preserve">
+-2.5 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-2.9 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-4.0 (90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-4.0 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-4.0 (75)</t>
   </si>
   <si>
     <t xml:space="preserve">2021-01-12</t>
@@ -975,6 +1028,9 @@
     <t xml:space="preserve">-2.5 (75)</t>
   </si>
   <si>
+    <t xml:space="preserve">-4.0 (80)</t>
+  </si>
+  <si>
     <t xml:space="preserve">-4.0 (85)</t>
   </si>
   <si>
@@ -1013,9 +1069,6 @@
 +0.1 (75)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.1 (75)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2021-04-11</t>
   </si>
   <si>
@@ -1455,9 +1508,6 @@
 &lt;forecast&gt; (&lt;confidence&gt;)
 Example: +0.3 (80)
 Do NOT use any information published after 08 October 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.1 (85)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.1 (80)</t>
@@ -7961,75 +8011,75 @@
         <v>161</v>
       </c>
       <c r="L61" t="n">
-        <v>0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="M61" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="N61" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
       <c r="O61" t="n">
-        <v>0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="P61" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="Q61" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
       <c r="R61" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S61" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="T61" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="U61" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="V61" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W61" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="X61" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="Y61" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="Z61" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="AA61" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AB61" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AC61" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="AD61" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AE61" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AF61" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C62" t="n">
         <v>0.1</v>
@@ -8038,7 +8088,7 @@
         <v>50</v>
       </c>
       <c r="E62" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F62" t="n">
         <v>0.1</v>
@@ -8047,7 +8097,7 @@
         <v>50</v>
       </c>
       <c r="H62" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I62" t="n">
         <v>0.1</v>
@@ -8056,7 +8106,7 @@
         <v>50</v>
       </c>
       <c r="K62" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L62" t="n">
         <v>0.1</v>
@@ -8065,7 +8115,7 @@
         <v>55</v>
       </c>
       <c r="N62" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="O62" t="n">
         <v>0.1</v>
@@ -8074,7 +8124,7 @@
         <v>55</v>
       </c>
       <c r="Q62" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="R62" t="n">
         <v>0.1</v>
@@ -8083,7 +8133,7 @@
         <v>65</v>
       </c>
       <c r="T62" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="U62" t="n">
         <v>0.1</v>
@@ -8092,7 +8142,7 @@
         <v>65</v>
       </c>
       <c r="W62" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="X62" t="n">
         <v>0.1</v>
@@ -8101,7 +8151,7 @@
         <v>60</v>
       </c>
       <c r="Z62" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AA62" t="n">
         <v>0.1</v>
@@ -8110,7 +8160,7 @@
         <v>60</v>
       </c>
       <c r="AC62" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AD62" t="n">
         <v>0.1</v>
@@ -8119,15 +8169,15 @@
         <v>60</v>
       </c>
       <c r="AF62" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C63" t="n">
         <v>0.1</v>
@@ -8136,7 +8186,7 @@
         <v>30</v>
       </c>
       <c r="E63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F63" t="n">
         <v>0.1</v>
@@ -8145,7 +8195,7 @@
         <v>30</v>
       </c>
       <c r="H63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I63" t="n">
         <v>0.1</v>
@@ -8154,7 +8204,7 @@
         <v>30</v>
       </c>
       <c r="K63" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L63" t="n">
         <v>0.1</v>
@@ -8163,7 +8213,7 @@
         <v>40</v>
       </c>
       <c r="N63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="O63" t="n">
         <v>0.1</v>
@@ -8172,7 +8222,7 @@
         <v>40</v>
       </c>
       <c r="Q63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="R63" t="n">
         <v>0.1</v>
@@ -8181,7 +8231,7 @@
         <v>40</v>
       </c>
       <c r="T63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="U63" t="n">
         <v>0.1</v>
@@ -8190,7 +8240,7 @@
         <v>40</v>
       </c>
       <c r="W63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="X63" t="n">
         <v>0.1</v>
@@ -8199,7 +8249,7 @@
         <v>40</v>
       </c>
       <c r="Z63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AA63" t="n">
         <v>0.1</v>
@@ -8208,7 +8258,7 @@
         <v>40</v>
       </c>
       <c r="AC63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AD63" t="n">
         <v>0.1</v>
@@ -8217,15 +8267,15 @@
         <v>40</v>
       </c>
       <c r="AF63" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B64" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C64" t="n">
         <v>-6</v>
@@ -8234,7 +8284,7 @@
         <v>85</v>
       </c>
       <c r="E64" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F64" t="n">
         <v>-6</v>
@@ -8243,7 +8293,7 @@
         <v>85</v>
       </c>
       <c r="H64" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I64" t="n">
         <v>-6</v>
@@ -8252,7 +8302,7 @@
         <v>85</v>
       </c>
       <c r="K64" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="L64" t="n">
         <v>-6</v>
@@ -8261,7 +8311,7 @@
         <v>90</v>
       </c>
       <c r="N64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O64" t="n">
         <v>-6</v>
@@ -8270,7 +8320,7 @@
         <v>90</v>
       </c>
       <c r="Q64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R64" t="n">
         <v>-6</v>
@@ -8279,7 +8329,7 @@
         <v>90</v>
       </c>
       <c r="T64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U64" t="n">
         <v>-6</v>
@@ -8288,7 +8338,7 @@
         <v>90</v>
       </c>
       <c r="W64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X64" t="n">
         <v>-6</v>
@@ -8297,7 +8347,7 @@
         <v>90</v>
       </c>
       <c r="Z64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA64" t="n">
         <v>-6</v>
@@ -8306,7 +8356,7 @@
         <v>90</v>
       </c>
       <c r="AC64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD64" t="n">
         <v>-6</v>
@@ -8315,15 +8365,15 @@
         <v>90</v>
       </c>
       <c r="AF64" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B65" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C65" t="n">
         <v>-15</v>
@@ -8332,7 +8382,7 @@
         <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F65" t="n">
         <v>-15</v>
@@ -8341,7 +8391,7 @@
         <v>60</v>
       </c>
       <c r="H65" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I65" t="n">
         <v>-15</v>
@@ -8350,7 +8400,7 @@
         <v>60</v>
       </c>
       <c r="K65" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="L65" t="n">
         <v>-20</v>
@@ -8359,7 +8409,7 @@
         <v>70</v>
       </c>
       <c r="N65" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="O65" t="n">
         <v>-20</v>
@@ -8368,7 +8418,7 @@
         <v>70</v>
       </c>
       <c r="Q65" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="R65" t="n">
         <v>-16</v>
@@ -8377,7 +8427,7 @@
         <v>30</v>
       </c>
       <c r="T65" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="U65" t="n">
         <v>-15</v>
@@ -8386,7 +8436,7 @@
         <v>30</v>
       </c>
       <c r="W65" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="X65" t="n">
         <v>-20</v>
@@ -8395,7 +8445,7 @@
         <v>40</v>
       </c>
       <c r="Z65" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AA65" t="n">
         <v>-20</v>
@@ -8404,7 +8454,7 @@
         <v>40</v>
       </c>
       <c r="AC65" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AD65" t="n">
         <v>-20</v>
@@ -8413,15 +8463,15 @@
         <v>40</v>
       </c>
       <c r="AF65" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C66" t="n">
         <v>-15</v>
@@ -8430,7 +8480,7 @@
         <v>75</v>
       </c>
       <c r="E66" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F66" t="n">
         <v>-15</v>
@@ -8439,7 +8489,7 @@
         <v>75</v>
       </c>
       <c r="H66" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I66" t="n">
         <v>-15</v>
@@ -8448,7 +8498,7 @@
         <v>75</v>
       </c>
       <c r="K66" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L66" t="n">
         <v>-15</v>
@@ -8457,7 +8507,7 @@
         <v>90</v>
       </c>
       <c r="N66" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="O66" t="n">
         <v>-15</v>
@@ -8466,7 +8516,7 @@
         <v>90</v>
       </c>
       <c r="Q66" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="R66" t="n">
         <v>-15</v>
@@ -8475,7 +8525,7 @@
         <v>70</v>
       </c>
       <c r="T66" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="U66" t="n">
         <v>-15</v>
@@ -8484,7 +8534,7 @@
         <v>70</v>
       </c>
       <c r="W66" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="X66" t="n">
         <v>-15</v>
@@ -8493,7 +8543,7 @@
         <v>40</v>
       </c>
       <c r="Z66" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="AA66" t="n">
         <v>-15</v>
@@ -8502,7 +8552,7 @@
         <v>40</v>
       </c>
       <c r="AC66" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="AD66" t="n">
         <v>-15</v>
@@ -8511,15 +8561,15 @@
         <v>40</v>
       </c>
       <c r="AF66" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B67" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C67" t="n">
         <v>-13.8</v>
@@ -8528,7 +8578,7 @@
         <v>70</v>
       </c>
       <c r="E67" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F67" t="n">
         <v>-15</v>
@@ -8537,7 +8587,7 @@
         <v>70</v>
       </c>
       <c r="H67" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I67" t="n">
         <v>-15</v>
@@ -8546,7 +8596,7 @@
         <v>70</v>
       </c>
       <c r="K67" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="L67" t="n">
         <v>-14</v>
@@ -8555,7 +8605,7 @@
         <v>80</v>
       </c>
       <c r="N67" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O67" t="n">
         <v>-14</v>
@@ -8564,7 +8614,7 @@
         <v>80</v>
       </c>
       <c r="Q67" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="R67" t="n">
         <v>-14</v>
@@ -8573,7 +8623,7 @@
         <v>85</v>
       </c>
       <c r="T67" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="U67" t="n">
         <v>-14</v>
@@ -8582,7 +8632,7 @@
         <v>85</v>
       </c>
       <c r="W67" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="X67" t="n">
         <v>-14</v>
@@ -8591,7 +8641,7 @@
         <v>75</v>
       </c>
       <c r="Z67" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AA67" t="n">
         <v>-14</v>
@@ -8600,7 +8650,7 @@
         <v>75</v>
       </c>
       <c r="AC67" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AD67" t="n">
         <v>-14</v>
@@ -8609,113 +8659,113 @@
         <v>75</v>
       </c>
       <c r="AF67" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B68" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C68" t="n">
         <v>16</v>
       </c>
       <c r="D68" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E68" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F68" t="n">
         <v>16</v>
       </c>
       <c r="G68" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="H68" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="I68" t="n">
         <v>16</v>
       </c>
       <c r="J68" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="K68" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="L68" t="n">
         <v>16</v>
       </c>
       <c r="M68" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="N68" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="O68" t="n">
         <v>16</v>
       </c>
       <c r="P68" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="Q68" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="R68" t="n">
-        <v>16</v>
+        <v>15.7</v>
       </c>
       <c r="S68" t="n">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="T68" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="U68" t="n">
-        <v>16</v>
+        <v>15.7</v>
       </c>
       <c r="V68" t="n">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="W68" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="X68" t="n">
         <v>16</v>
       </c>
       <c r="Y68" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="Z68" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="AA68" t="n">
         <v>16</v>
       </c>
       <c r="AB68" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AC68" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="AD68" t="n">
         <v>16</v>
       </c>
       <c r="AE68" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AF68" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B69" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C69" t="n">
         <v>16</v>
@@ -8724,7 +8774,7 @@
         <v>80</v>
       </c>
       <c r="E69" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F69" t="n">
         <v>16</v>
@@ -8733,7 +8783,7 @@
         <v>80</v>
       </c>
       <c r="H69" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="I69" t="n">
         <v>16</v>
@@ -8742,7 +8792,7 @@
         <v>80</v>
       </c>
       <c r="K69" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="L69" t="n">
         <v>16</v>
@@ -8751,7 +8801,7 @@
         <v>85</v>
       </c>
       <c r="N69" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="O69" t="n">
         <v>16</v>
@@ -8760,7 +8810,7 @@
         <v>85</v>
       </c>
       <c r="Q69" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="R69" t="n">
         <v>16</v>
@@ -8769,7 +8819,7 @@
         <v>85</v>
       </c>
       <c r="T69" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="U69" t="n">
         <v>16</v>
@@ -8778,7 +8828,7 @@
         <v>85</v>
       </c>
       <c r="W69" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="X69" t="n">
         <v>16</v>
@@ -8787,7 +8837,7 @@
         <v>80</v>
       </c>
       <c r="Z69" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="AA69" t="n">
         <v>16</v>
@@ -8796,7 +8846,7 @@
         <v>80</v>
       </c>
       <c r="AC69" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="AD69" t="n">
         <v>16</v>
@@ -8805,60 +8855,60 @@
         <v>80</v>
       </c>
       <c r="AF69" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B70" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C70" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D70" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E70" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="F70" t="n">
-        <v>16</v>
+        <v>15.7</v>
       </c>
       <c r="G70" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H70" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="I70" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J70" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K70" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="L70" t="n">
         <v>16</v>
       </c>
       <c r="M70" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="N70" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="O70" t="n">
         <v>16</v>
       </c>
       <c r="P70" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="Q70" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="R70" t="n">
         <v>16</v>
@@ -8867,7 +8917,7 @@
         <v>85</v>
       </c>
       <c r="T70" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="U70" t="n">
         <v>16</v>
@@ -8876,16 +8926,16 @@
         <v>85</v>
       </c>
       <c r="W70" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="X70" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Y70" t="n">
         <v>85</v>
       </c>
       <c r="Z70" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AA70" t="n">
         <v>16</v>
@@ -8894,7 +8944,7 @@
         <v>85</v>
       </c>
       <c r="AC70" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="AD70" t="n">
         <v>16</v>
@@ -8903,158 +8953,158 @@
         <v>85</v>
       </c>
       <c r="AF70" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B71" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C71" t="n">
-        <v>-4</v>
+        <v>-4.2</v>
       </c>
       <c r="D71" t="n">
+        <v>65</v>
+      </c>
+      <c r="E71" t="s">
+        <v>241</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="G71" t="n">
+        <v>65</v>
+      </c>
+      <c r="H71" t="s">
+        <v>242</v>
+      </c>
+      <c r="I71" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="J71" t="n">
+        <v>65</v>
+      </c>
+      <c r="K71" t="s">
+        <v>242</v>
+      </c>
+      <c r="L71" t="n">
+        <v>-5.8</v>
+      </c>
+      <c r="M71" t="n">
+        <v>70</v>
+      </c>
+      <c r="N71" t="s">
+        <v>243</v>
+      </c>
+      <c r="O71" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="P71" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>242</v>
+      </c>
+      <c r="R71" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="S71" t="n">
+        <v>65</v>
+      </c>
+      <c r="T71" t="s">
+        <v>244</v>
+      </c>
+      <c r="U71" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="V71" t="n">
+        <v>65</v>
+      </c>
+      <c r="W71" t="s">
+        <v>244</v>
+      </c>
+      <c r="X71" t="n">
+        <v>-5.4</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>65</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="AB71" t="n">
         <v>60</v>
       </c>
-      <c r="E71" t="s">
-        <v>233</v>
-      </c>
-      <c r="F71" t="n">
-        <v>-4</v>
-      </c>
-      <c r="G71" t="n">
-        <v>60</v>
-      </c>
-      <c r="H71" t="s">
-        <v>233</v>
-      </c>
-      <c r="I71" t="n">
-        <v>-4</v>
-      </c>
-      <c r="J71" t="n">
-        <v>60</v>
-      </c>
-      <c r="K71" t="s">
-        <v>233</v>
-      </c>
-      <c r="L71" t="n">
-        <v>-6</v>
-      </c>
-      <c r="M71" t="n">
-        <v>40</v>
-      </c>
-      <c r="N71" t="s">
-        <v>234</v>
-      </c>
-      <c r="O71" t="n">
-        <v>-6</v>
-      </c>
-      <c r="P71" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>234</v>
-      </c>
-      <c r="R71" t="n">
-        <v>-4</v>
-      </c>
-      <c r="S71" t="n">
-        <v>50</v>
-      </c>
-      <c r="T71" t="s">
-        <v>235</v>
-      </c>
-      <c r="U71" t="n">
-        <v>-4</v>
-      </c>
-      <c r="V71" t="n">
-        <v>50</v>
-      </c>
-      <c r="W71" t="s">
-        <v>235</v>
-      </c>
-      <c r="X71" t="n">
-        <v>-4.2</v>
-      </c>
-      <c r="Y71" t="n">
-        <v>40</v>
-      </c>
-      <c r="Z71" t="s">
-        <v>236</v>
-      </c>
-      <c r="AA71" t="n">
-        <v>-4.2</v>
-      </c>
-      <c r="AB71" t="n">
-        <v>40</v>
-      </c>
       <c r="AC71" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="AD71" t="n">
-        <v>-4.2</v>
+        <v>-5.4</v>
       </c>
       <c r="AE71" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="AF71" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="B72" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="C72" t="n">
-        <v>-4</v>
+        <v>-2.5</v>
       </c>
       <c r="D72" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E72" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="F72" t="n">
-        <v>-4</v>
+        <v>-2.9</v>
       </c>
       <c r="G72" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H72" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="I72" t="n">
         <v>-4</v>
       </c>
       <c r="J72" t="n">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="K72" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="L72" t="n">
         <v>-4</v>
       </c>
       <c r="M72" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="N72" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="O72" t="n">
         <v>-4</v>
       </c>
       <c r="P72" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="Q72" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="R72" t="n">
         <v>-4</v>
@@ -9063,7 +9113,7 @@
         <v>75</v>
       </c>
       <c r="T72" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="U72" t="n">
         <v>-4</v>
@@ -9072,42 +9122,42 @@
         <v>75</v>
       </c>
       <c r="W72" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="X72" t="n">
         <v>-4</v>
       </c>
       <c r="Y72" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="Z72" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="AA72" t="n">
         <v>-4</v>
       </c>
       <c r="AB72" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AC72" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="AD72" t="n">
         <v>-4</v>
       </c>
       <c r="AE72" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AF72" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="C73" t="n">
         <v>-2.5</v>
@@ -9116,7 +9166,7 @@
         <v>75</v>
       </c>
       <c r="E73" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="F73" t="n">
         <v>-2.5</v>
@@ -9125,7 +9175,7 @@
         <v>75</v>
       </c>
       <c r="H73" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="I73" t="n">
         <v>-2.5</v>
@@ -9134,7 +9184,7 @@
         <v>75</v>
       </c>
       <c r="K73" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="L73" t="n">
         <v>-4</v>
@@ -9143,7 +9193,7 @@
         <v>80</v>
       </c>
       <c r="N73" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="O73" t="n">
         <v>-4</v>
@@ -9152,7 +9202,7 @@
         <v>80</v>
       </c>
       <c r="Q73" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="R73" t="n">
         <v>-4</v>
@@ -9161,7 +9211,7 @@
         <v>85</v>
       </c>
       <c r="T73" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="U73" t="n">
         <v>-4</v>
@@ -9170,7 +9220,7 @@
         <v>85</v>
       </c>
       <c r="W73" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="X73" t="n">
         <v>-4</v>
@@ -9179,7 +9229,7 @@
         <v>85</v>
       </c>
       <c r="Z73" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="AA73" t="n">
         <v>-4</v>
@@ -9188,7 +9238,7 @@
         <v>85</v>
       </c>
       <c r="AC73" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="AD73" t="n">
         <v>-4</v>
@@ -9197,15 +9247,15 @@
         <v>85</v>
       </c>
       <c r="AF73" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B74" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
@@ -9214,7 +9264,7 @@
         <v>50</v>
       </c>
       <c r="E74" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -9223,7 +9273,7 @@
         <v>50</v>
       </c>
       <c r="H74" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
@@ -9232,7 +9282,7 @@
         <v>50</v>
       </c>
       <c r="K74" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="L74" t="n">
         <v>-0.3</v>
@@ -9241,7 +9291,7 @@
         <v>60</v>
       </c>
       <c r="N74" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="O74" t="n">
         <v>-0.3</v>
@@ -9250,7 +9300,7 @@
         <v>60</v>
       </c>
       <c r="Q74" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="R74" t="n">
         <v>-0.1</v>
@@ -9259,7 +9309,7 @@
         <v>65</v>
       </c>
       <c r="T74" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="U74" t="n">
         <v>-0.1</v>
@@ -9268,7 +9318,7 @@
         <v>65</v>
       </c>
       <c r="W74" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="X74" t="n">
         <v>-0.3</v>
@@ -9277,7 +9327,7 @@
         <v>60</v>
       </c>
       <c r="Z74" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="AA74" t="n">
         <v>-0.3</v>
@@ -9286,7 +9336,7 @@
         <v>60</v>
       </c>
       <c r="AC74" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="AD74" t="n">
         <v>-0.3</v>
@@ -9295,15 +9345,15 @@
         <v>60</v>
       </c>
       <c r="AF74" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="C75" t="n">
         <v>0.3</v>
@@ -9339,7 +9389,7 @@
         <v>75</v>
       </c>
       <c r="N75" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="O75" t="n">
         <v>0.1</v>
@@ -9348,7 +9398,7 @@
         <v>75</v>
       </c>
       <c r="Q75" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="R75" t="n">
         <v>0.3</v>
@@ -9398,10 +9448,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="B76" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="C76" t="n">
         <v>0.3</v>
@@ -9455,7 +9505,7 @@
         <v>85</v>
       </c>
       <c r="T76" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="U76" t="n">
         <v>0.7</v>
@@ -9464,7 +9514,7 @@
         <v>85</v>
       </c>
       <c r="W76" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="X76" t="n">
         <v>0.2</v>
@@ -9496,10 +9546,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="B77" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="C77" t="n">
         <v>0.9</v>
@@ -9508,7 +9558,7 @@
         <v>75</v>
       </c>
       <c r="E77" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="F77" t="n">
         <v>1</v>
@@ -9517,7 +9567,7 @@
         <v>75</v>
       </c>
       <c r="H77" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="I77" t="n">
         <v>1</v>
@@ -9526,7 +9576,7 @@
         <v>75</v>
       </c>
       <c r="K77" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="L77" t="n">
         <v>0.5</v>
@@ -9535,7 +9585,7 @@
         <v>75</v>
       </c>
       <c r="N77" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="O77" t="n">
         <v>0.5</v>
@@ -9544,7 +9594,7 @@
         <v>75</v>
       </c>
       <c r="Q77" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="R77" t="n">
         <v>1.1</v>
@@ -9553,7 +9603,7 @@
         <v>75</v>
       </c>
       <c r="T77" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="U77" t="n">
         <v>1.1</v>
@@ -9562,7 +9612,7 @@
         <v>75</v>
       </c>
       <c r="W77" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="X77" t="n">
         <v>1.1</v>
@@ -9571,7 +9621,7 @@
         <v>85</v>
       </c>
       <c r="Z77" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="AA77" t="n">
         <v>1.1</v>
@@ -9580,7 +9630,7 @@
         <v>85</v>
       </c>
       <c r="AC77" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="AD77" t="n">
         <v>1.1</v>
@@ -9589,15 +9639,15 @@
         <v>85</v>
       </c>
       <c r="AF77" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="B78" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="C78" t="n">
         <v>0.8</v>
@@ -9606,7 +9656,7 @@
         <v>85</v>
       </c>
       <c r="E78" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="F78" t="n">
         <v>0.8</v>
@@ -9615,7 +9665,7 @@
         <v>85</v>
       </c>
       <c r="H78" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="I78" t="n">
         <v>0.8</v>
@@ -9624,7 +9674,7 @@
         <v>85</v>
       </c>
       <c r="K78" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="L78" t="n">
         <v>0.8</v>
@@ -9633,7 +9683,7 @@
         <v>85</v>
       </c>
       <c r="N78" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="O78" t="n">
         <v>0.8</v>
@@ -9642,7 +9692,7 @@
         <v>85</v>
       </c>
       <c r="Q78" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="R78" t="n">
         <v>0.8</v>
@@ -9651,7 +9701,7 @@
         <v>75</v>
       </c>
       <c r="T78" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="U78" t="n">
         <v>0.8</v>
@@ -9660,7 +9710,7 @@
         <v>75</v>
       </c>
       <c r="W78" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="X78" t="n">
         <v>0.9</v>
@@ -9669,7 +9719,7 @@
         <v>85</v>
       </c>
       <c r="Z78" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="AA78" t="n">
         <v>0.8</v>
@@ -9678,7 +9728,7 @@
         <v>85</v>
       </c>
       <c r="AC78" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="AD78" t="n">
         <v>0.8</v>
@@ -9687,15 +9737,15 @@
         <v>85</v>
       </c>
       <c r="AF78" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="B79" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="C79" t="n">
         <v>0.9</v>
@@ -9704,7 +9754,7 @@
         <v>85</v>
       </c>
       <c r="E79" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="F79" t="n">
         <v>0.9</v>
@@ -9713,7 +9763,7 @@
         <v>85</v>
       </c>
       <c r="H79" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="I79" t="n">
         <v>0.9</v>
@@ -9722,7 +9772,7 @@
         <v>85</v>
       </c>
       <c r="K79" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="L79" t="n">
         <v>0.9</v>
@@ -9731,7 +9781,7 @@
         <v>85</v>
       </c>
       <c r="N79" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="O79" t="n">
         <v>0.9</v>
@@ -9740,7 +9790,7 @@
         <v>85</v>
       </c>
       <c r="Q79" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="R79" t="n">
         <v>1</v>
@@ -9749,7 +9799,7 @@
         <v>90</v>
       </c>
       <c r="T79" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="U79" t="n">
         <v>1</v>
@@ -9758,7 +9808,7 @@
         <v>90</v>
       </c>
       <c r="W79" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="X79" t="n">
         <v>1.1</v>
@@ -9767,7 +9817,7 @@
         <v>90</v>
       </c>
       <c r="Z79" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="AA79" t="n">
         <v>1.1</v>
@@ -9776,7 +9826,7 @@
         <v>90</v>
       </c>
       <c r="AC79" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="AD79" t="n">
         <v>1.1</v>
@@ -9785,15 +9835,15 @@
         <v>90</v>
       </c>
       <c r="AF79" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="B80" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="C80" t="n">
         <v>2.3</v>
@@ -9802,7 +9852,7 @@
         <v>75</v>
       </c>
       <c r="E80" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="F80" t="n">
         <v>2.3</v>
@@ -9811,7 +9861,7 @@
         <v>75</v>
       </c>
       <c r="H80" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="I80" t="n">
         <v>2.3</v>
@@ -9820,7 +9870,7 @@
         <v>75</v>
       </c>
       <c r="K80" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="L80" t="n">
         <v>2.5</v>
@@ -9829,7 +9879,7 @@
         <v>75</v>
       </c>
       <c r="N80" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="O80" t="n">
         <v>2.5</v>
@@ -9838,7 +9888,7 @@
         <v>75</v>
       </c>
       <c r="Q80" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="R80" t="n">
         <v>2.5</v>
@@ -9847,7 +9897,7 @@
         <v>75</v>
       </c>
       <c r="T80" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="U80" t="n">
         <v>2.5</v>
@@ -9856,7 +9906,7 @@
         <v>75</v>
       </c>
       <c r="W80" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="X80" t="n">
         <v>1.5</v>
@@ -9865,7 +9915,7 @@
         <v>75</v>
       </c>
       <c r="Z80" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="AA80" t="n">
         <v>1.5</v>
@@ -9874,7 +9924,7 @@
         <v>75</v>
       </c>
       <c r="AC80" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="AD80" t="n">
         <v>1.5</v>
@@ -9883,15 +9933,15 @@
         <v>75</v>
       </c>
       <c r="AF80" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="B81" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="C81" t="n">
         <v>2.3</v>
@@ -9900,7 +9950,7 @@
         <v>75</v>
       </c>
       <c r="E81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="F81" t="n">
         <v>2.3</v>
@@ -9909,7 +9959,7 @@
         <v>75</v>
       </c>
       <c r="H81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="I81" t="n">
         <v>2.3</v>
@@ -9918,7 +9968,7 @@
         <v>75</v>
       </c>
       <c r="K81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="L81" t="n">
         <v>2.3</v>
@@ -9927,7 +9977,7 @@
         <v>75</v>
       </c>
       <c r="N81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="O81" t="n">
         <v>2.3</v>
@@ -9936,7 +9986,7 @@
         <v>75</v>
       </c>
       <c r="Q81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="R81" t="n">
         <v>2.3</v>
@@ -9945,7 +9995,7 @@
         <v>75</v>
       </c>
       <c r="T81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="U81" t="n">
         <v>2.3</v>
@@ -9954,7 +10004,7 @@
         <v>75</v>
       </c>
       <c r="W81" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="X81" t="n">
         <v>1.5</v>
@@ -9963,7 +10013,7 @@
         <v>85</v>
       </c>
       <c r="Z81" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="AA81" t="n">
         <v>1.5</v>
@@ -9972,7 +10022,7 @@
         <v>85</v>
       </c>
       <c r="AC81" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="AD81" t="n">
         <v>2.3</v>
@@ -9981,15 +10031,15 @@
         <v>85</v>
       </c>
       <c r="AF81" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="B82" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="C82" t="n">
         <v>2.1</v>
@@ -9998,7 +10048,7 @@
         <v>90</v>
       </c>
       <c r="E82" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="F82" t="n">
         <v>2.5</v>
@@ -10007,7 +10057,7 @@
         <v>85</v>
       </c>
       <c r="H82" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="I82" t="n">
         <v>2.5</v>
@@ -10016,7 +10066,7 @@
         <v>85</v>
       </c>
       <c r="K82" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="L82" t="n">
         <v>2.7</v>
@@ -10025,7 +10075,7 @@
         <v>80</v>
       </c>
       <c r="N82" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="O82" t="n">
         <v>2.7</v>
@@ -10034,7 +10084,7 @@
         <v>80</v>
       </c>
       <c r="Q82" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="R82" t="n">
         <v>2.5</v>
@@ -10043,7 +10093,7 @@
         <v>85</v>
       </c>
       <c r="T82" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="U82" t="n">
         <v>2.5</v>
@@ -10052,7 +10102,7 @@
         <v>85</v>
       </c>
       <c r="W82" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="X82" t="n">
         <v>2.5</v>
@@ -10061,7 +10111,7 @@
         <v>85</v>
       </c>
       <c r="Z82" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="AA82" t="n">
         <v>2.5</v>
@@ -10070,7 +10120,7 @@
         <v>85</v>
       </c>
       <c r="AC82" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="AD82" t="n">
         <v>2.5</v>
@@ -10079,15 +10129,15 @@
         <v>85</v>
       </c>
       <c r="AF82" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="B83" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="C83" t="n">
         <v>0.6</v>
@@ -10123,7 +10173,7 @@
         <v>80</v>
       </c>
       <c r="N83" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="O83" t="n">
         <v>0.7</v>
@@ -10132,7 +10182,7 @@
         <v>80</v>
       </c>
       <c r="Q83" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="R83" t="n">
         <v>0.6</v>
@@ -10141,7 +10191,7 @@
         <v>75</v>
       </c>
       <c r="T83" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="U83" t="n">
         <v>0.6</v>
@@ -10150,7 +10200,7 @@
         <v>75</v>
       </c>
       <c r="W83" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="X83" t="n">
         <v>0.8</v>
@@ -10159,7 +10209,7 @@
         <v>80</v>
       </c>
       <c r="Z83" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AA83" t="n">
         <v>0.8</v>
@@ -10168,7 +10218,7 @@
         <v>80</v>
       </c>
       <c r="AC83" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AD83" t="n">
         <v>0.8</v>
@@ -10177,15 +10227,15 @@
         <v>80</v>
       </c>
       <c r="AF83" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="B84" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="C84" t="n">
         <v>0.6</v>
@@ -10194,7 +10244,7 @@
         <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="F84" t="n">
         <v>0.6</v>
@@ -10203,7 +10253,7 @@
         <v>65</v>
       </c>
       <c r="H84" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="I84" t="n">
         <v>0.6</v>
@@ -10212,7 +10262,7 @@
         <v>65</v>
       </c>
       <c r="K84" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="L84" t="n">
         <v>0.7</v>
@@ -10221,7 +10271,7 @@
         <v>70</v>
       </c>
       <c r="N84" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="O84" t="n">
         <v>0.7</v>
@@ -10230,7 +10280,7 @@
         <v>70</v>
       </c>
       <c r="Q84" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="R84" t="n">
         <v>0.7</v>
@@ -10239,7 +10289,7 @@
         <v>65</v>
       </c>
       <c r="T84" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="U84" t="n">
         <v>0.7</v>
@@ -10248,7 +10298,7 @@
         <v>65</v>
       </c>
       <c r="W84" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="X84" t="n">
         <v>0.7</v>
@@ -10257,7 +10307,7 @@
         <v>60</v>
       </c>
       <c r="Z84" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="AA84" t="n">
         <v>0.7</v>
@@ -10266,7 +10316,7 @@
         <v>60</v>
       </c>
       <c r="AC84" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="AD84" t="n">
         <v>0.7</v>
@@ -10275,15 +10325,15 @@
         <v>60</v>
       </c>
       <c r="AF84" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="B85" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="C85" t="n">
         <v>0.75</v>
@@ -10292,7 +10342,7 @@
         <v>85</v>
       </c>
       <c r="E85" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="F85" t="n">
         <v>0.75</v>
@@ -10301,7 +10351,7 @@
         <v>85</v>
       </c>
       <c r="H85" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="I85" t="n">
         <v>0.75</v>
@@ -10310,7 +10360,7 @@
         <v>85</v>
       </c>
       <c r="K85" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="L85" t="n">
         <v>0.6</v>
@@ -10319,7 +10369,7 @@
         <v>75</v>
       </c>
       <c r="N85" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="O85" t="n">
         <v>0.6</v>
@@ -10328,7 +10378,7 @@
         <v>75</v>
       </c>
       <c r="Q85" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="R85" t="n">
         <v>0.6</v>
@@ -10337,7 +10387,7 @@
         <v>75</v>
       </c>
       <c r="T85" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="U85" t="n">
         <v>0.6</v>
@@ -10346,7 +10396,7 @@
         <v>75</v>
       </c>
       <c r="W85" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="X85" t="n">
         <v>0.7</v>
@@ -10355,7 +10405,7 @@
         <v>85</v>
       </c>
       <c r="Z85" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="AA85" t="n">
         <v>0.6</v>
@@ -10373,15 +10423,15 @@
         <v>85</v>
       </c>
       <c r="AF85" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="B86" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="C86" t="n">
         <v>0.3</v>
@@ -10476,10 +10526,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="B87" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="C87" t="n">
         <v>0.3</v>
@@ -10488,7 +10538,7 @@
         <v>40</v>
       </c>
       <c r="E87" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="F87" t="n">
         <v>0.3</v>
@@ -10497,7 +10547,7 @@
         <v>40</v>
       </c>
       <c r="H87" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="I87" t="n">
         <v>0.3</v>
@@ -10506,7 +10556,7 @@
         <v>40</v>
       </c>
       <c r="K87" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="L87" t="n">
         <v>0.3</v>
@@ -10533,7 +10583,7 @@
         <v>50</v>
       </c>
       <c r="T87" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="U87" t="n">
         <v>0.3</v>
@@ -10542,7 +10592,7 @@
         <v>50</v>
       </c>
       <c r="W87" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="X87" t="n">
         <v>0.3</v>
@@ -10551,7 +10601,7 @@
         <v>40</v>
       </c>
       <c r="Z87" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="AA87" t="n">
         <v>0.3</v>
@@ -10560,7 +10610,7 @@
         <v>40</v>
       </c>
       <c r="AC87" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="AD87" t="n">
         <v>0.3</v>
@@ -10569,15 +10619,15 @@
         <v>40</v>
       </c>
       <c r="AF87" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="B88" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="C88" t="n">
         <v>0.3</v>
@@ -10586,7 +10636,7 @@
         <v>55</v>
       </c>
       <c r="E88" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="F88" t="n">
         <v>0.3</v>
@@ -10595,7 +10645,7 @@
         <v>55</v>
       </c>
       <c r="H88" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="I88" t="n">
         <v>0.3</v>
@@ -10604,7 +10654,7 @@
         <v>55</v>
       </c>
       <c r="K88" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="L88" t="n">
         <v>0.3</v>
@@ -10672,10 +10722,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="B89" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="C89" t="n">
         <v>0.2</v>
@@ -10738,7 +10788,7 @@
         <v>65</v>
       </c>
       <c r="W89" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="X89" t="n">
         <v>0.2</v>
@@ -10770,10 +10820,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="B90" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C90" t="n">
         <v>0.3</v>
@@ -10868,10 +10918,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="B91" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="C91" t="n">
         <v>0.3</v>
@@ -10966,10 +11016,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="B92" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="C92" t="n">
         <v>0.2</v>
@@ -10996,7 +11046,7 @@
         <v>65</v>
       </c>
       <c r="K92" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="L92" t="n">
         <v>0.2</v>
@@ -11064,10 +11114,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="B93" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="C93" t="n">
         <v>0.3</v>
@@ -11162,10 +11212,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="B94" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="C94" t="n">
         <v>0.2</v>
@@ -11260,10 +11310,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="B95" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="C95" t="n">
         <v>0.1</v>
@@ -11272,7 +11322,7 @@
         <v>45</v>
       </c>
       <c r="E95" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="F95" t="n">
         <v>0.1</v>
@@ -11281,7 +11331,7 @@
         <v>45</v>
       </c>
       <c r="H95" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="I95" t="n">
         <v>0.1</v>
@@ -11290,7 +11340,7 @@
         <v>45</v>
       </c>
       <c r="K95" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="L95" t="n">
         <v>0.1</v>
@@ -11299,7 +11349,7 @@
         <v>55</v>
       </c>
       <c r="N95" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="O95" t="n">
         <v>0.1</v>
@@ -11308,7 +11358,7 @@
         <v>55</v>
       </c>
       <c r="Q95" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="R95" t="n">
         <v>0.1</v>
@@ -11317,7 +11367,7 @@
         <v>60</v>
       </c>
       <c r="T95" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="U95" t="n">
         <v>0.1</v>
@@ -11326,7 +11376,7 @@
         <v>60</v>
       </c>
       <c r="W95" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="X95" t="n">
         <v>0.1</v>
@@ -11335,7 +11385,7 @@
         <v>60</v>
       </c>
       <c r="Z95" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AA95" t="n">
         <v>0.1</v>
@@ -11344,7 +11394,7 @@
         <v>60</v>
       </c>
       <c r="AC95" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AD95" t="n">
         <v>0.1</v>
@@ -11353,15 +11403,15 @@
         <v>60</v>
       </c>
       <c r="AF95" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="B96" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="C96" t="n">
         <v>0.1</v>
@@ -11370,7 +11420,7 @@
         <v>60</v>
       </c>
       <c r="E96" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F96" t="n">
         <v>0.1</v>
@@ -11379,7 +11429,7 @@
         <v>60</v>
       </c>
       <c r="H96" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I96" t="n">
         <v>0.1</v>
@@ -11388,7 +11438,7 @@
         <v>60</v>
       </c>
       <c r="K96" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="L96" t="n">
         <v>0.1</v>
@@ -11397,7 +11447,7 @@
         <v>65</v>
       </c>
       <c r="N96" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O96" t="n">
         <v>0.1</v>
@@ -11406,7 +11456,7 @@
         <v>65</v>
       </c>
       <c r="Q96" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R96" t="n">
         <v>0.1</v>
@@ -11415,7 +11465,7 @@
         <v>55</v>
       </c>
       <c r="T96" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="U96" t="n">
         <v>0.1</v>
@@ -11424,7 +11474,7 @@
         <v>55</v>
       </c>
       <c r="W96" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="X96" t="n">
         <v>0.1</v>
@@ -11433,7 +11483,7 @@
         <v>60</v>
       </c>
       <c r="Z96" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AA96" t="n">
         <v>0.1</v>
@@ -11442,7 +11492,7 @@
         <v>60</v>
       </c>
       <c r="AC96" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AD96" t="n">
         <v>0.1</v>
@@ -11451,15 +11501,15 @@
         <v>60</v>
       </c>
       <c r="AF96" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="B97" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="C97" t="n">
         <v>0.2</v>
@@ -11554,10 +11604,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="B98" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="C98" t="n">
         <v>0.1</v>
@@ -11566,7 +11616,7 @@
         <v>65</v>
       </c>
       <c r="E98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F98" t="n">
         <v>0.1</v>
@@ -11575,7 +11625,7 @@
         <v>65</v>
       </c>
       <c r="H98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I98" t="n">
         <v>0.1</v>
@@ -11584,7 +11634,7 @@
         <v>65</v>
       </c>
       <c r="K98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L98" t="n">
         <v>0.1</v>
@@ -11593,7 +11643,7 @@
         <v>65</v>
       </c>
       <c r="N98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O98" t="n">
         <v>0.1</v>
@@ -11602,7 +11652,7 @@
         <v>65</v>
       </c>
       <c r="Q98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R98" t="n">
         <v>0.2</v>
@@ -11629,7 +11679,7 @@
         <v>65</v>
       </c>
       <c r="Z98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AA98" t="n">
         <v>0.1</v>
@@ -11638,7 +11688,7 @@
         <v>65</v>
       </c>
       <c r="AC98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AD98" t="n">
         <v>0.1</v>
@@ -11647,15 +11697,15 @@
         <v>65</v>
       </c>
       <c r="AF98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="B99" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="C99" t="n">
         <v>0.2</v>
@@ -11750,10 +11800,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="B100" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="C100" t="n">
         <v>0.2</v>
@@ -11789,7 +11839,7 @@
         <v>90</v>
       </c>
       <c r="N100" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="O100" t="n">
         <v>0.2</v>
@@ -11798,7 +11848,7 @@
         <v>90</v>
       </c>
       <c r="Q100" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="R100" t="n">
         <v>0.2</v>
@@ -11848,10 +11898,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="B101" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="C101" t="n">
         <v>0.1</v>
@@ -11860,7 +11910,7 @@
         <v>65</v>
       </c>
       <c r="E101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F101" t="n">
         <v>0.1</v>
@@ -11869,7 +11919,7 @@
         <v>65</v>
       </c>
       <c r="H101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I101" t="n">
         <v>0.1</v>
@@ -11878,7 +11928,7 @@
         <v>65</v>
       </c>
       <c r="K101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L101" t="n">
         <v>0.1</v>
@@ -11887,7 +11937,7 @@
         <v>65</v>
       </c>
       <c r="N101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O101" t="n">
         <v>0.1</v>
@@ -11896,7 +11946,7 @@
         <v>65</v>
       </c>
       <c r="Q101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R101" t="n">
         <v>0.1</v>
@@ -11905,7 +11955,7 @@
         <v>65</v>
       </c>
       <c r="T101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="U101" t="n">
         <v>0.1</v>
@@ -11914,7 +11964,7 @@
         <v>65</v>
       </c>
       <c r="W101" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="X101" t="n">
         <v>0.2</v>
@@ -11946,10 +11996,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="B102" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="C102" t="n">
         <v>0.1</v>
@@ -11958,7 +12008,7 @@
         <v>75</v>
       </c>
       <c r="E102" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="F102" t="n">
         <v>0.1</v>
@@ -11967,7 +12017,7 @@
         <v>75</v>
       </c>
       <c r="H102" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="I102" t="n">
         <v>0.1</v>
@@ -11976,7 +12026,7 @@
         <v>75</v>
       </c>
       <c r="K102" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="L102" t="n">
         <v>0.2</v>
@@ -12044,10 +12094,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="B103" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="C103" t="n">
         <v>0.2</v>
@@ -12142,10 +12192,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="B104" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="C104" t="n">
         <v>0.1</v>
@@ -12154,7 +12204,7 @@
         <v>50</v>
       </c>
       <c r="E104" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F104" t="n">
         <v>0.1</v>
@@ -12163,7 +12213,7 @@
         <v>50</v>
       </c>
       <c r="H104" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I104" t="n">
         <v>0.1</v>
@@ -12172,7 +12222,7 @@
         <v>50</v>
       </c>
       <c r="K104" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L104" t="n">
         <v>0.1</v>
@@ -12181,7 +12231,7 @@
         <v>50</v>
       </c>
       <c r="N104" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="O104" t="n">
         <v>0.1</v>
@@ -12190,7 +12240,7 @@
         <v>50</v>
       </c>
       <c r="Q104" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="R104" t="n">
         <v>0.1</v>
@@ -12199,7 +12249,7 @@
         <v>55</v>
       </c>
       <c r="T104" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="U104" t="n">
         <v>0.1</v>
@@ -12208,7 +12258,7 @@
         <v>55</v>
       </c>
       <c r="W104" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="X104" t="n">
         <v>0.1</v>
@@ -12217,7 +12267,7 @@
         <v>45</v>
       </c>
       <c r="Z104" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="AA104" t="n">
         <v>0.1</v>
@@ -12226,7 +12276,7 @@
         <v>45</v>
       </c>
       <c r="AC104" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="AD104" t="n">
         <v>0.1</v>
@@ -12235,15 +12285,15 @@
         <v>45</v>
       </c>
       <c r="AF104" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="B105" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C105" t="n">
         <v>0.1</v>
@@ -12252,7 +12302,7 @@
         <v>70</v>
       </c>
       <c r="E105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="F105" t="n">
         <v>0.1</v>
@@ -12261,7 +12311,7 @@
         <v>70</v>
       </c>
       <c r="H105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="I105" t="n">
         <v>0.1</v>
@@ -12270,7 +12320,7 @@
         <v>70</v>
       </c>
       <c r="K105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="L105" t="n">
         <v>0.1</v>
@@ -12279,7 +12329,7 @@
         <v>70</v>
       </c>
       <c r="N105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="O105" t="n">
         <v>0.1</v>
@@ -12288,7 +12338,7 @@
         <v>70</v>
       </c>
       <c r="Q105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="R105" t="n">
         <v>0.1</v>
@@ -12297,7 +12347,7 @@
         <v>70</v>
       </c>
       <c r="T105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="U105" t="n">
         <v>0.1</v>
@@ -12306,7 +12356,7 @@
         <v>70</v>
       </c>
       <c r="W105" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="X105" t="n">
         <v>0.1</v>
@@ -12315,7 +12365,7 @@
         <v>75</v>
       </c>
       <c r="Z105" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="AA105" t="n">
         <v>0.1</v>
@@ -12324,7 +12374,7 @@
         <v>75</v>
       </c>
       <c r="AC105" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="AD105" t="n">
         <v>0.1</v>
@@ -12333,15 +12383,15 @@
         <v>75</v>
       </c>
       <c r="AF105" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="B106" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="C106" t="n">
         <v>0.1</v>
@@ -12350,7 +12400,7 @@
         <v>85</v>
       </c>
       <c r="E106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="F106" t="n">
         <v>0.1</v>
@@ -12359,7 +12409,7 @@
         <v>85</v>
       </c>
       <c r="H106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="I106" t="n">
         <v>0.1</v>
@@ -12368,7 +12418,7 @@
         <v>85</v>
       </c>
       <c r="K106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="L106" t="n">
         <v>0.1</v>
@@ -12377,7 +12427,7 @@
         <v>80</v>
       </c>
       <c r="N106" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="O106" t="n">
         <v>0.1</v>
@@ -12386,7 +12436,7 @@
         <v>80</v>
       </c>
       <c r="Q106" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="R106" t="n">
         <v>0.1</v>
@@ -12395,7 +12445,7 @@
         <v>85</v>
       </c>
       <c r="T106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="U106" t="n">
         <v>0.1</v>
@@ -12404,7 +12454,7 @@
         <v>85</v>
       </c>
       <c r="W106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="X106" t="n">
         <v>0.1</v>
@@ -12413,7 +12463,7 @@
         <v>85</v>
       </c>
       <c r="Z106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="AA106" t="n">
         <v>0.1</v>
@@ -12422,7 +12472,7 @@
         <v>85</v>
       </c>
       <c r="AC106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="AD106" t="n">
         <v>0.1</v>
@@ -12431,15 +12481,15 @@
         <v>85</v>
       </c>
       <c r="AF106" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="B107" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="C107" t="n">
         <v>0.1</v>
@@ -12448,7 +12498,7 @@
         <v>65</v>
       </c>
       <c r="E107" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F107" t="n">
         <v>0.1</v>
@@ -12457,7 +12507,7 @@
         <v>65</v>
       </c>
       <c r="H107" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I107" t="n">
         <v>0.1</v>
@@ -12466,7 +12516,7 @@
         <v>65</v>
       </c>
       <c r="K107" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L107" t="n">
         <v>0</v>
@@ -12475,7 +12525,7 @@
         <v>70</v>
       </c>
       <c r="N107" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="O107" t="n">
         <v>0</v>
@@ -12484,7 +12534,7 @@
         <v>70</v>
       </c>
       <c r="Q107" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="R107" t="n">
         <v>0.1</v>
@@ -12493,7 +12543,7 @@
         <v>70</v>
       </c>
       <c r="T107" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="U107" t="n">
         <v>0.1</v>
@@ -12502,7 +12552,7 @@
         <v>70</v>
       </c>
       <c r="W107" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="X107" t="n">
         <v>0</v>
@@ -12511,7 +12561,7 @@
         <v>60</v>
       </c>
       <c r="Z107" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="AA107" t="n">
         <v>0</v>
@@ -12520,7 +12570,7 @@
         <v>60</v>
       </c>
       <c r="AC107" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="AD107" t="n">
         <v>0</v>
@@ -12529,15 +12579,15 @@
         <v>60</v>
       </c>
       <c r="AF107" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="B108" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="C108" t="n">
         <v>-0.1</v>
@@ -12546,7 +12596,7 @@
         <v>65</v>
       </c>
       <c r="E108" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="F108" t="n">
         <v>-0.1</v>
@@ -12555,7 +12605,7 @@
         <v>65</v>
       </c>
       <c r="H108" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="I108" t="n">
         <v>-0.1</v>
@@ -12564,7 +12614,7 @@
         <v>65</v>
       </c>
       <c r="K108" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="L108" t="n">
         <v>0</v>
@@ -12573,7 +12623,7 @@
         <v>75</v>
       </c>
       <c r="N108" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="O108" t="n">
         <v>0</v>
@@ -12582,7 +12632,7 @@
         <v>75</v>
       </c>
       <c r="Q108" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="R108" t="n">
         <v>0</v>
@@ -12591,7 +12641,7 @@
         <v>75</v>
       </c>
       <c r="T108" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="U108" t="n">
         <v>0</v>
@@ -12600,7 +12650,7 @@
         <v>75</v>
       </c>
       <c r="W108" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="X108" t="n">
         <v>-0.1</v>
@@ -12609,7 +12659,7 @@
         <v>65</v>
       </c>
       <c r="Z108" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="AA108" t="n">
         <v>-0.1</v>
@@ -12618,7 +12668,7 @@
         <v>65</v>
       </c>
       <c r="AC108" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="AD108" t="n">
         <v>-0.1</v>
@@ -12627,15 +12677,15 @@
         <v>65</v>
       </c>
       <c r="AF108" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="B109" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="C109" t="n">
         <v>0.2</v>
@@ -12671,7 +12721,7 @@
         <v>90</v>
       </c>
       <c r="N109" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="O109" t="n">
         <v>0.2</v>
@@ -12680,7 +12730,7 @@
         <v>90</v>
       </c>
       <c r="Q109" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="R109" t="n">
         <v>0.2</v>
@@ -12730,10 +12780,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="B110" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="C110" t="n">
         <v>0.1</v>
@@ -12742,7 +12792,7 @@
         <v>65</v>
       </c>
       <c r="E110" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F110" t="n">
         <v>0.1</v>
@@ -12751,7 +12801,7 @@
         <v>65</v>
       </c>
       <c r="H110" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I110" t="n">
         <v>0.1</v>
@@ -12760,7 +12810,7 @@
         <v>65</v>
       </c>
       <c r="K110" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L110" t="n">
         <v>0.2</v>
@@ -12805,7 +12855,7 @@
         <v>65</v>
       </c>
       <c r="Z110" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AA110" t="n">
         <v>0.1</v>
@@ -12814,7 +12864,7 @@
         <v>65</v>
       </c>
       <c r="AC110" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AD110" t="n">
         <v>0.1</v>
@@ -12823,15 +12873,15 @@
         <v>65</v>
       </c>
       <c r="AF110" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="B111" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="C111" t="n">
         <v>0.2</v>
@@ -12926,10 +12976,10 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="B112" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="C112" t="n">
         <v>0.2</v>
@@ -12938,7 +12988,7 @@
         <v>90</v>
       </c>
       <c r="E112" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="F112" t="n">
         <v>0.2</v>
@@ -12947,7 +12997,7 @@
         <v>90</v>
       </c>
       <c r="H112" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="I112" t="n">
         <v>0.2</v>
@@ -12956,7 +13006,7 @@
         <v>90</v>
       </c>
       <c r="K112" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="L112" t="n">
         <v>0.2</v>
@@ -12965,7 +13015,7 @@
         <v>90</v>
       </c>
       <c r="N112" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="O112" t="n">
         <v>0.2</v>
@@ -12974,7 +13024,7 @@
         <v>90</v>
       </c>
       <c r="Q112" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="R112" t="n">
         <v>0.2</v>
@@ -13001,7 +13051,7 @@
         <v>100</v>
       </c>
       <c r="Z112" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="AA112" t="n">
         <v>0.2</v>
@@ -13010,7 +13060,7 @@
         <v>100</v>
       </c>
       <c r="AC112" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="AD112" t="n">
         <v>0.2</v>
@@ -13019,15 +13069,15 @@
         <v>100</v>
       </c>
       <c r="AF112" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="B113" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="C113" t="n">
         <v>0.1</v>
@@ -13036,7 +13086,7 @@
         <v>65</v>
       </c>
       <c r="E113" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F113" t="n">
         <v>0.1</v>
@@ -13045,7 +13095,7 @@
         <v>65</v>
       </c>
       <c r="H113" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I113" t="n">
         <v>0.1</v>
@@ -13054,7 +13104,7 @@
         <v>65</v>
       </c>
       <c r="K113" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L113" t="n">
         <v>0.2</v>
@@ -13063,7 +13113,7 @@
         <v>55</v>
       </c>
       <c r="N113" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="O113" t="n">
         <v>0.2</v>
@@ -13072,7 +13122,7 @@
         <v>55</v>
       </c>
       <c r="Q113" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="R113" t="n">
         <v>0.2</v>
@@ -13122,10 +13172,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="B114" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="C114" t="n">
         <v>0.1</v>
@@ -13134,7 +13184,7 @@
         <v>75</v>
       </c>
       <c r="E114" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="F114" t="n">
         <v>0.1</v>
@@ -13143,7 +13193,7 @@
         <v>75</v>
       </c>
       <c r="H114" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="I114" t="n">
         <v>0.1</v>
@@ -13152,7 +13202,7 @@
         <v>75</v>
       </c>
       <c r="K114" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="L114" t="n">
         <v>0.1</v>
@@ -13161,7 +13211,7 @@
         <v>65</v>
       </c>
       <c r="N114" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O114" t="n">
         <v>0.1</v>
@@ -13170,7 +13220,7 @@
         <v>65</v>
       </c>
       <c r="Q114" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R114" t="n">
         <v>0.1</v>
@@ -13179,7 +13229,7 @@
         <v>75</v>
       </c>
       <c r="T114" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="U114" t="n">
         <v>0.1</v>
@@ -13188,7 +13238,7 @@
         <v>75</v>
       </c>
       <c r="W114" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="X114" t="n">
         <v>0.2</v>
@@ -13220,10 +13270,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="B115" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="C115" t="n">
         <v>0.1</v>
@@ -13232,7 +13282,7 @@
         <v>70</v>
       </c>
       <c r="E115" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="F115" t="n">
         <v>0.1</v>
@@ -13241,7 +13291,7 @@
         <v>70</v>
       </c>
       <c r="H115" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="I115" t="n">
         <v>0.1</v>
@@ -13250,7 +13300,7 @@
         <v>70</v>
       </c>
       <c r="K115" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="L115" t="n">
         <v>0.1</v>
@@ -13259,7 +13309,7 @@
         <v>65</v>
       </c>
       <c r="N115" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O115" t="n">
         <v>0.1</v>
@@ -13268,7 +13318,7 @@
         <v>65</v>
       </c>
       <c r="Q115" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R115" t="n">
         <v>0.1</v>
@@ -13277,7 +13327,7 @@
         <v>70</v>
       </c>
       <c r="T115" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="U115" t="n">
         <v>0.1</v>
@@ -13286,7 +13336,7 @@
         <v>70</v>
       </c>
       <c r="W115" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="X115" t="n">
         <v>0.1</v>
@@ -13295,7 +13345,7 @@
         <v>80</v>
       </c>
       <c r="Z115" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="AA115" t="n">
         <v>0.1</v>
@@ -13304,7 +13354,7 @@
         <v>80</v>
       </c>
       <c r="AC115" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="AD115" t="n">
         <v>0.1</v>
@@ -13313,15 +13363,15 @@
         <v>80</v>
       </c>
       <c r="AF115" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="B116" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="C116" t="n">
         <v>0.2</v>
@@ -13416,10 +13466,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="B117" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="C117" t="n">
         <v>0.2</v>
@@ -13514,10 +13564,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="B118" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="C118" t="n">
         <v>0.3</v>
@@ -13612,10 +13662,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="B119" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="C119" t="n">
         <v>0.1</v>
@@ -13624,7 +13674,7 @@
         <v>60</v>
       </c>
       <c r="E119" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F119" t="n">
         <v>0.1</v>
@@ -13633,7 +13683,7 @@
         <v>60</v>
       </c>
       <c r="H119" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I119" t="n">
         <v>0.1</v>
@@ -13642,7 +13692,7 @@
         <v>60</v>
       </c>
       <c r="K119" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="L119" t="n">
         <v>0.1</v>
@@ -13651,7 +13701,7 @@
         <v>65</v>
       </c>
       <c r="N119" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O119" t="n">
         <v>0.1</v>
@@ -13660,7 +13710,7 @@
         <v>65</v>
       </c>
       <c r="Q119" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R119" t="n">
         <v>0.1</v>
@@ -13669,7 +13719,7 @@
         <v>55</v>
       </c>
       <c r="T119" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="U119" t="n">
         <v>0.1</v>
@@ -13678,7 +13728,7 @@
         <v>55</v>
       </c>
       <c r="W119" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="X119" t="n">
         <v>0</v>
@@ -13687,7 +13737,7 @@
         <v>65</v>
       </c>
       <c r="Z119" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="AA119" t="n">
         <v>0</v>
@@ -13696,7 +13746,7 @@
         <v>65</v>
       </c>
       <c r="AC119" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="AD119" t="n">
         <v>0</v>
@@ -13705,15 +13755,15 @@
         <v>65</v>
       </c>
       <c r="AF119" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="B120" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="C120" t="n">
         <v>0.1</v>
@@ -13722,7 +13772,7 @@
         <v>65</v>
       </c>
       <c r="E120" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F120" t="n">
         <v>0.1</v>
@@ -13731,7 +13781,7 @@
         <v>65</v>
       </c>
       <c r="H120" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I120" t="n">
         <v>0.1</v>
@@ -13740,7 +13790,7 @@
         <v>65</v>
       </c>
       <c r="K120" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L120" t="n">
         <v>0</v>
@@ -13749,7 +13799,7 @@
         <v>70</v>
       </c>
       <c r="N120" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="O120" t="n">
         <v>0</v>
@@ -13758,7 +13808,7 @@
         <v>70</v>
       </c>
       <c r="Q120" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="R120" t="n">
         <v>0</v>
@@ -13767,7 +13817,7 @@
         <v>65</v>
       </c>
       <c r="T120" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="U120" t="n">
         <v>0</v>
@@ -13776,7 +13826,7 @@
         <v>65</v>
       </c>
       <c r="W120" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="X120" t="n">
         <v>0.1</v>
@@ -13785,7 +13835,7 @@
         <v>60</v>
       </c>
       <c r="Z120" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AA120" t="n">
         <v>0.1</v>
@@ -13794,7 +13844,7 @@
         <v>60</v>
       </c>
       <c r="AC120" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AD120" t="n">
         <v>0.1</v>
@@ -13803,15 +13853,15 @@
         <v>60</v>
       </c>
       <c r="AF120" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
       <c r="B121" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="C121" t="n">
         <v>0.1</v>
@@ -13820,7 +13870,7 @@
         <v>70</v>
       </c>
       <c r="E121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="F121" t="n">
         <v>0.1</v>
@@ -13829,7 +13879,7 @@
         <v>70</v>
       </c>
       <c r="H121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="I121" t="n">
         <v>0.1</v>
@@ -13838,7 +13888,7 @@
         <v>70</v>
       </c>
       <c r="K121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="L121" t="n">
         <v>0.1</v>
@@ -13847,7 +13897,7 @@
         <v>70</v>
       </c>
       <c r="N121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="O121" t="n">
         <v>0.1</v>
@@ -13856,7 +13906,7 @@
         <v>70</v>
       </c>
       <c r="Q121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="R121" t="n">
         <v>0.1</v>
@@ -13865,7 +13915,7 @@
         <v>70</v>
       </c>
       <c r="T121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="U121" t="n">
         <v>0.1</v>
@@ -13874,7 +13924,7 @@
         <v>70</v>
       </c>
       <c r="W121" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="X121" t="n">
         <v>0.1</v>
@@ -13883,7 +13933,7 @@
         <v>75</v>
       </c>
       <c r="Z121" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="AA121" t="n">
         <v>0.1</v>
@@ -13892,7 +13942,7 @@
         <v>75</v>
       </c>
       <c r="AC121" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="AD121" t="n">
         <v>0.1</v>
@@ -13901,15 +13951,15 @@
         <v>75</v>
       </c>
       <c r="AF121" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="B122" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
       <c r="C122" t="n">
         <v>0.2</v>
@@ -13945,7 +13995,7 @@
         <v>65</v>
       </c>
       <c r="N122" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O122" t="n">
         <v>0.1</v>
@@ -13954,7 +14004,7 @@
         <v>65</v>
       </c>
       <c r="Q122" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R122" t="n">
         <v>0.2</v>
@@ -13981,7 +14031,7 @@
         <v>75</v>
       </c>
       <c r="Z122" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="AA122" t="n">
         <v>0.1</v>
@@ -13990,7 +14040,7 @@
         <v>75</v>
       </c>
       <c r="AC122" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="AD122" t="n">
         <v>0.1</v>
@@ -13999,15 +14049,15 @@
         <v>75</v>
       </c>
       <c r="AF122" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="B123" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="C123" t="n">
         <v>0.2</v>
@@ -14102,10 +14152,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="B124" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="C124" t="n">
         <v>0.2</v>
@@ -14200,10 +14250,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="B125" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="C125" t="n">
         <v>0.1</v>
@@ -14212,7 +14262,7 @@
         <v>65</v>
       </c>
       <c r="E125" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F125" t="n">
         <v>0.1</v>
@@ -14221,7 +14271,7 @@
         <v>65</v>
       </c>
       <c r="H125" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I125" t="n">
         <v>0.1</v>
@@ -14230,7 +14280,7 @@
         <v>65</v>
       </c>
       <c r="K125" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L125" t="n">
         <v>0.2</v>
@@ -14298,10 +14348,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="B126" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="C126" t="n">
         <v>0.1</v>
@@ -14310,7 +14360,7 @@
         <v>70</v>
       </c>
       <c r="E126" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="F126" t="n">
         <v>0.1</v>
@@ -14319,7 +14369,7 @@
         <v>70</v>
       </c>
       <c r="H126" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="I126" t="n">
         <v>0.1</v>
@@ -14328,7 +14378,7 @@
         <v>70</v>
       </c>
       <c r="K126" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="L126" t="n">
         <v>0.1</v>
@@ -14337,7 +14387,7 @@
         <v>60</v>
       </c>
       <c r="N126" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="O126" t="n">
         <v>0.1</v>
@@ -14346,7 +14396,7 @@
         <v>60</v>
       </c>
       <c r="Q126" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="R126" t="n">
         <v>-0.1</v>
@@ -14355,7 +14405,7 @@
         <v>75</v>
       </c>
       <c r="T126" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="U126" t="n">
         <v>-0.1</v>
@@ -14364,7 +14414,7 @@
         <v>75</v>
       </c>
       <c r="W126" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="X126" t="n">
         <v>0.1</v>
@@ -14373,7 +14423,7 @@
         <v>65</v>
       </c>
       <c r="Z126" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AA126" t="n">
         <v>0.1</v>
@@ -14382,7 +14432,7 @@
         <v>65</v>
       </c>
       <c r="AC126" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AD126" t="n">
         <v>0.1</v>
@@ -14391,15 +14441,15 @@
         <v>65</v>
       </c>
       <c r="AF126" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="B127" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="C127"/>
       <c r="D127"/>
@@ -14411,7 +14461,7 @@
         <v>80</v>
       </c>
       <c r="H127" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="I127" t="n">
         <v>0.2</v>
@@ -14459,7 +14509,7 @@
         <v>85</v>
       </c>
       <c r="Z127" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="AA127" t="n">
         <v>0.1</v>
@@ -14468,7 +14518,7 @@
         <v>85</v>
       </c>
       <c r="AC127" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="AD127" t="n">
         <v>0.1</v>
@@ -14477,15 +14527,15 @@
         <v>85</v>
       </c>
       <c r="AF127" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="B128" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="C128" t="n">
         <v>0.2</v>
@@ -14580,10 +14630,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="B129" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="C129" t="n">
         <v>0.2</v>
@@ -14678,10 +14728,10 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="B130" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="C130" t="n">
         <v>0.2</v>
@@ -14776,10 +14826,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="B131" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C131" t="n">
         <v>0.2</v>
@@ -14815,7 +14865,7 @@
         <v>65</v>
       </c>
       <c r="N131" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O131" t="n">
         <v>0.1</v>
@@ -14824,7 +14874,7 @@
         <v>65</v>
       </c>
       <c r="Q131" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R131" t="n">
         <v>0.1</v>
@@ -14833,7 +14883,7 @@
         <v>60</v>
       </c>
       <c r="T131" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="U131" t="n">
         <v>0.1</v>
@@ -14842,7 +14892,7 @@
         <v>60</v>
       </c>
       <c r="W131" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="X131" t="n">
         <v>0.1</v>
@@ -14851,7 +14901,7 @@
         <v>65</v>
       </c>
       <c r="Z131" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AA131" t="n">
         <v>0.1</v>
@@ -14860,7 +14910,7 @@
         <v>65</v>
       </c>
       <c r="AC131" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AD131" t="n">
         <v>0.1</v>
@@ -14869,7 +14919,7 @@
         <v>65</v>
       </c>
       <c r="AF131" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>